<commit_message>
fix : jenkins build failure
</commit_message>
<xml_diff>
--- a/ML/kmeans_test.xlsx
+++ b/ML/kmeans_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ssafy\PJT2\S06P22D104\ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92317179-F53A-4D93-9FEF-68ADC2B51232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70148FE5-6F6A-4DD5-81F4-A96E97F14110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12960" yWindow="2265" windowWidth="11910" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1635" yWindow="2280" windowWidth="11910" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kmeans_train" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
   <si>
     <t>성별</t>
   </si>
@@ -171,6 +171,18 @@
   </si>
   <si>
     <t>향수id</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>All Time</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>봄/여름</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>가을/겨울</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -878,6 +890,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -895,15 +916,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1263,113 +1275,113 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="9" style="16"/>
+    <col min="1" max="7" width="9" style="10"/>
     <col min="9" max="9" width="12.375" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="15">
-        <v>0</v>
-      </c>
-      <c r="B2" s="16">
-        <v>0</v>
-      </c>
-      <c r="C2" s="16">
-        <v>0</v>
-      </c>
-      <c r="D2" s="16">
-        <v>0</v>
-      </c>
-      <c r="E2" s="16">
-        <v>1</v>
-      </c>
-      <c r="F2" s="16">
-        <v>1</v>
-      </c>
-      <c r="G2" s="16" t="s">
+      <c r="A2" s="9">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0</v>
+      </c>
+      <c r="D2" s="10">
+        <v>0</v>
+      </c>
+      <c r="E2" s="10">
+        <v>1</v>
+      </c>
+      <c r="F2" s="10">
+        <v>1</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="15">
-        <v>1</v>
-      </c>
-      <c r="B3" s="16">
-        <v>0</v>
-      </c>
-      <c r="C3" s="16">
-        <v>0</v>
-      </c>
-      <c r="D3" s="16">
-        <v>0</v>
-      </c>
-      <c r="E3" s="16">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10">
         <v>3</v>
       </c>
-      <c r="F3" s="16">
-        <v>1</v>
-      </c>
-      <c r="G3" s="16" t="s">
+      <c r="F3" s="10">
+        <v>1</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="11"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="14"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="15">
-        <v>2</v>
-      </c>
-      <c r="B4" s="16">
-        <v>1</v>
-      </c>
-      <c r="C4" s="16">
-        <v>1</v>
-      </c>
-      <c r="D4" s="16">
-        <v>1</v>
-      </c>
-      <c r="E4" s="16">
-        <v>2</v>
-      </c>
-      <c r="F4" s="16">
-        <v>2</v>
-      </c>
-      <c r="G4" s="16" t="s">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10">
+        <v>1</v>
+      </c>
+      <c r="C4" s="10">
+        <v>1</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10">
+        <v>2</v>
+      </c>
+      <c r="F4" s="10">
+        <v>2</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>36</v>
       </c>
       <c r="I4" s="1">
@@ -1378,30 +1390,32 @@
       <c r="J4" s="2">
         <v>1</v>
       </c>
-      <c r="K4" s="2"/>
+      <c r="K4" s="2">
+        <v>2</v>
+      </c>
       <c r="L4" s="2"/>
       <c r="M4" s="3"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="15">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" s="16">
-        <v>1</v>
-      </c>
-      <c r="C5" s="16">
-        <v>1</v>
-      </c>
-      <c r="D5" s="16">
-        <v>1</v>
-      </c>
-      <c r="E5" s="16">
+      <c r="B5" s="10">
+        <v>1</v>
+      </c>
+      <c r="C5" s="10">
+        <v>1</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10">
         <v>3</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="10">
         <v>3</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="10" t="s">
         <v>37</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -1410,30 +1424,32 @@
       <c r="J5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="L5" s="2"/>
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="15">
+      <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="16">
-        <v>0</v>
-      </c>
-      <c r="C6" s="16">
-        <v>0</v>
-      </c>
-      <c r="D6" s="16">
-        <v>2</v>
-      </c>
-      <c r="E6" s="16">
-        <v>2</v>
-      </c>
-      <c r="F6" s="16">
-        <v>2</v>
-      </c>
-      <c r="G6" s="16" t="s">
+      <c r="B6" s="10">
+        <v>0</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0</v>
+      </c>
+      <c r="D6" s="10">
+        <v>2</v>
+      </c>
+      <c r="E6" s="10">
+        <v>2</v>
+      </c>
+      <c r="F6" s="10">
+        <v>2</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>38</v>
       </c>
       <c r="I6" s="1"/>
@@ -1443,34 +1459,34 @@
       <c r="M6" s="3"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="15">
+      <c r="A7" s="9">
         <v>5</v>
       </c>
-      <c r="B7" s="16">
-        <v>1</v>
-      </c>
-      <c r="C7" s="16">
-        <v>2</v>
-      </c>
-      <c r="D7" s="16">
+      <c r="B7" s="10">
+        <v>1</v>
+      </c>
+      <c r="C7" s="10">
+        <v>2</v>
+      </c>
+      <c r="D7" s="10">
         <v>3</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="10">
         <v>4</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="10">
         <v>4</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="14"/>
+      <c r="I7" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="17"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I8" s="1">
@@ -1506,13 +1522,13 @@
       <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I11" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="14"/>
+      <c r="I11" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="17"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I12" s="1">
@@ -1521,27 +1537,19 @@
       <c r="J12" s="2">
         <v>1</v>
       </c>
-      <c r="K12" s="2">
-        <v>2</v>
-      </c>
-      <c r="L12" s="2">
-        <v>3</v>
-      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
       <c r="M12" s="3"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I13" s="1" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
       <c r="M13" s="3"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1552,26 +1560,26 @@
       <c r="M14" s="3"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I15" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="14"/>
+      <c r="I15" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="17"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I16" s="1">
         <v>0</v>
       </c>
-      <c r="J16" s="2" t="s">
-        <v>33</v>
+      <c r="J16" s="2">
+        <v>1</v>
       </c>
       <c r="K16" s="2">
         <v>2</v>
       </c>
       <c r="L16" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M16" s="3"/>
     </row>
@@ -1588,7 +1596,7 @@
       <c r="L17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M17" s="17"/>
+      <c r="M17" s="11"/>
     </row>
     <row r="18" spans="9:13" x14ac:dyDescent="0.3">
       <c r="I18" s="1" t="s">
@@ -1603,7 +1611,7 @@
       <c r="L18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M18" s="17"/>
+      <c r="M18" s="11"/>
     </row>
     <row r="19" spans="9:13" x14ac:dyDescent="0.3">
       <c r="I19" s="1"/>
@@ -1613,13 +1621,13 @@
       <c r="M19" s="3"/>
     </row>
     <row r="20" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I20" s="12" t="s">
+      <c r="I20" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="14"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="17"/>
     </row>
     <row r="21" spans="9:13" x14ac:dyDescent="0.3">
       <c r="I21" s="1">
@@ -1768,13 +1776,13 @@
       <c r="G3" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="11"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="14"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -1890,13 +1898,13 @@
       <c r="G7" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="14"/>
+      <c r="I7" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="17"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I8" s="1">
@@ -1932,13 +1940,13 @@
       <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I11" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="14"/>
+      <c r="I11" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="17"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I12" s="1">
@@ -1978,13 +1986,13 @@
       <c r="M14" s="3"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I15" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="14"/>
+      <c r="I15" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="17"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I16" s="1">
@@ -2039,13 +2047,13 @@
       <c r="M19" s="3"/>
     </row>
     <row r="20" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I20" s="12" t="s">
+      <c r="I20" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="14"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="17"/>
     </row>
     <row r="21" spans="9:13" x14ac:dyDescent="0.3">
       <c r="I21" s="1">

</xml_diff>